<commit_message>
Fix few bugs with data tables
</commit_message>
<xml_diff>
--- a/formshare/tests/resources/forms/data_columns/data_columns.xlsx
+++ b/formshare/tests/resources/forms/data_columns/data_columns.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="137">
   <si>
     <t xml:space="preserve">some notes</t>
   </si>
@@ -48,6 +48,9 @@
     <t xml:space="preserve">formshare_encrypted</t>
   </si>
   <si>
+    <t xml:space="preserve">formshare_unique</t>
+  </si>
+  <si>
     <t xml:space="preserve">formshare_ontological_term</t>
   </si>
   <si>
@@ -193,6 +196,12 @@
   </si>
   <si>
     <t xml:space="preserve">QST005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hr_qst_874b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique variable</t>
   </si>
   <si>
     <t xml:space="preserve">hr_qst_005</t>
@@ -637,13 +646,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="23.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.14"/>
@@ -652,16 +661,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="44.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="42.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="26.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="44.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="42.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.14"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,13 +704,13 @@
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -719,13 +728,16 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -736,314 +748,348 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-      <c r="M2" s="0"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="5"/>
+      <c r="L6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="0" t="s">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="0" t="s">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="I12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="L14" s="1"/>
-      <c r="Q14" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="R14" s="0" t="s">
-        <v>73</v>
-      </c>
+      <c r="M14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="R15" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="S15" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="0" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="C16" s="0" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>26</v>
+      <c r="E16" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>81</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I14" r:id="rId1" display="c_34835@agrovoc"/>
+    <hyperlink ref="J15" r:id="rId1" display="c_34835@agrovoc"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1068,7 +1114,7 @@
       <selection pane="bottomLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.14"/>
@@ -1080,7 +1126,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -1092,50 +1138,50 @@
         <v>4</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>101</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>201</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>101</v>
@@ -1143,16 +1189,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>202</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>101</v>
@@ -1160,16 +1206,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>301</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>201</v>
@@ -1180,16 +1226,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>302</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>201</v>
@@ -1200,16 +1246,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>303</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>201</v>
@@ -1220,16 +1266,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>304</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>201</v>
@@ -1240,16 +1286,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>305</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>202</v>
@@ -1260,16 +1306,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>306</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>202</v>
@@ -1280,16 +1326,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>307</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>202</v>
@@ -1300,16 +1346,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>308</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>202</v>
@@ -1320,16 +1366,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>309</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>202</v>
@@ -1340,16 +1386,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>310</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>202</v>
@@ -1360,16 +1406,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>311</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>202</v>
@@ -1380,124 +1426,124 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1522,11 +1568,11 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.15"/>
@@ -1535,18 +1581,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>